<commit_message>
tareas para prueba crime
</commit_message>
<xml_diff>
--- a/machine_learning/prueba/crimenes/2009 SQF File Spec_V2.xlsx
+++ b/machine_learning/prueba/crimenes/2009 SQF File Spec_V2.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braulio\Documents\ADL\03_Desafíos y Pruebas\Pruebas\Módulo 3 - ML\Prueba 3\prueba\crimenes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braulio\Documents\ADL\desafio-latam-tareas-BA-TP\machine_learning\prueba\crimenes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4845DE77-9C42-4979-B686-D1D928D4B1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E52A7CA-2420-47A4-BFEB-5CFE0756557E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1095" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SQF2009_File_Spec" sheetId="1" r:id="rId1"/>
     <sheet name="Value_Labels" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SQF2009_File_Spec!$A$4:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SQF2009_File_Spec!$A$4:$E$115</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Value_Labels!$A$5:$C$381</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">SQF2009_File_Spec!$A$1:$H$115</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Value_Labels!$A$1:$C$381</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="549">
   <si>
     <t>NYPD Stop Question Frisk Database  2009</t>
   </si>
@@ -1643,9 +1643,6 @@
   </si>
   <si>
     <t>ELIMINAR -  VARIABLE SUBJETIVA</t>
-  </si>
-  <si>
-    <t>MANTENER - VARIABLE VIOLENCIA</t>
   </si>
   <si>
     <t>ELIMINAR - VARIABLE "DISCRIMINACIÓN"</t>
@@ -2096,16 +2093,16 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2442,7 +2439,7 @@
   <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2492,7 +2489,7 @@
       <c r="D4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="45" t="s">
         <v>518</v>
       </c>
       <c r="F4" s="35"/>
@@ -2514,7 +2511,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2522,7 +2519,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="12">
-        <f>(B5+1)</f>
+        <f t="shared" ref="B6:B37" si="0">(B5+1)</f>
         <v>2</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -2532,7 +2529,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2540,7 +2537,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="12">
-        <f>(B6+1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -2550,7 +2547,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2558,7 +2555,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="12">
-        <f>(B7+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -2568,7 +2565,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2576,7 +2573,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="12">
-        <f>(B8+1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -2586,7 +2583,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2594,7 +2591,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="12">
-        <f>(B9+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -2612,7 +2609,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="12">
-        <f>(B10+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -2630,7 +2627,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="12">
-        <f>(B11+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -2648,7 +2645,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="12">
-        <f>(B12+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -2658,7 +2655,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2666,7 +2663,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="12">
-        <f>(B13+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -2676,7 +2673,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2684,7 +2681,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="12">
-        <f>(B14+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -2694,7 +2691,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2702,7 +2699,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="12">
-        <f>(B15+1)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -2712,7 +2709,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2720,7 +2717,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="12">
-        <f>(B16+1)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -2730,7 +2727,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2738,7 +2735,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="12">
-        <f>(B17+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2748,7 +2745,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2756,7 +2753,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="12">
-        <f>(B18+1)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2765,19 +2762,19 @@
       <c r="D19" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="43" t="s">
-        <v>539</v>
-      </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="E19" s="46" t="s">
+        <v>538</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="38" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="12">
-        <f>(B19+1)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -2787,7 +2784,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2795,7 +2792,7 @@
         <v>41</v>
       </c>
       <c r="B21" s="12">
-        <f>(B20+1)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -2813,7 +2810,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="12">
-        <f>(B21+1)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -2823,7 +2820,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2831,7 +2828,7 @@
         <v>45</v>
       </c>
       <c r="B23" s="12">
-        <f>(B22+1)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -2841,7 +2838,7 @@
         <v>9</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2849,7 +2846,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="12">
-        <f>(B23+1)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -2859,7 +2856,7 @@
         <v>18</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2867,7 +2864,7 @@
         <v>49</v>
       </c>
       <c r="B25" s="12">
-        <f>(B24+1)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -2885,7 +2882,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="12">
-        <f>(B25+1)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -2895,7 +2892,7 @@
         <v>9</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2903,7 +2900,7 @@
         <v>53</v>
       </c>
       <c r="B27" s="12">
-        <f>(B26+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2921,7 +2918,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="12">
-        <f>(B27+1)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -2931,7 +2928,7 @@
         <v>9</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2939,7 +2936,7 @@
         <v>57</v>
       </c>
       <c r="B29" s="12">
-        <f>(B28+1)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -2957,7 +2954,7 @@
         <v>59</v>
       </c>
       <c r="B30" s="12">
-        <f>(B29+1)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -2967,7 +2964,7 @@
         <v>9</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2975,7 +2972,7 @@
         <v>61</v>
       </c>
       <c r="B31" s="12">
-        <f>(B30+1)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -2985,7 +2982,7 @@
         <v>9</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2993,7 +2990,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="12">
-        <f>(B31+1)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -3003,7 +3000,7 @@
         <v>9</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -3011,7 +3008,7 @@
         <v>65</v>
       </c>
       <c r="B33" s="12">
-        <f>(B32+1)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -3021,7 +3018,7 @@
         <v>9</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3029,7 +3026,7 @@
         <v>67</v>
       </c>
       <c r="B34" s="12">
-        <f>(B33+1)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -3039,7 +3036,7 @@
         <v>9</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3047,7 +3044,7 @@
         <v>69</v>
       </c>
       <c r="B35" s="12">
-        <f>(B34+1)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -3057,7 +3054,7 @@
         <v>9</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3065,7 +3062,7 @@
         <v>71</v>
       </c>
       <c r="B36" s="12">
-        <f>(B35+1)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -3075,7 +3072,7 @@
         <v>9</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3083,7 +3080,7 @@
         <v>73</v>
       </c>
       <c r="B37" s="12">
-        <f>(B36+1)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3103,7 +3100,7 @@
         <v>75</v>
       </c>
       <c r="B38" s="12">
-        <f>(B37+1)</f>
+        <f t="shared" ref="B38:B69" si="1">(B37+1)</f>
         <v>34</v>
       </c>
       <c r="C38" s="11" t="s">
@@ -3123,7 +3120,7 @@
         <v>77</v>
       </c>
       <c r="B39" s="12">
-        <f>(B38+1)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -3143,7 +3140,7 @@
         <v>79</v>
       </c>
       <c r="B40" s="12">
-        <f>(B39+1)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -3163,7 +3160,7 @@
         <v>81</v>
       </c>
       <c r="B41" s="12">
-        <f>(B40+1)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C41" s="11" t="s">
@@ -3183,7 +3180,7 @@
         <v>83</v>
       </c>
       <c r="B42" s="12">
-        <f>(B41+1)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C42" s="11" t="s">
@@ -3203,7 +3200,7 @@
         <v>85</v>
       </c>
       <c r="B43" s="12">
-        <f>(B42+1)</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3223,7 +3220,7 @@
         <v>87</v>
       </c>
       <c r="B44" s="12">
-        <f>(B43+1)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -3243,7 +3240,7 @@
         <v>89</v>
       </c>
       <c r="B45" s="12">
-        <f>(B44+1)</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="C45" s="11" t="s">
@@ -3263,7 +3260,7 @@
         <v>91</v>
       </c>
       <c r="B46" s="12">
-        <f>(B45+1)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3281,7 +3278,7 @@
         <v>93</v>
       </c>
       <c r="B47" s="12">
-        <f>(B46+1)</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -3299,7 +3296,7 @@
         <v>95</v>
       </c>
       <c r="B48" s="12">
-        <f>(B47+1)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="C48" s="11" t="s">
@@ -3317,7 +3314,7 @@
         <v>97</v>
       </c>
       <c r="B49" s="12">
-        <f>(B48+1)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C49" s="11" t="s">
@@ -3327,7 +3324,7 @@
         <v>9</v>
       </c>
       <c r="E49" s="41" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3335,7 +3332,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="12">
-        <f>(B49+1)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="C50" s="11" t="s">
@@ -3353,7 +3350,7 @@
         <v>101</v>
       </c>
       <c r="B51" s="12">
-        <f>(B50+1)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="C51" s="11" t="s">
@@ -3371,7 +3368,7 @@
         <v>103</v>
       </c>
       <c r="B52" s="12">
-        <f>(B51+1)</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C52" s="11" t="s">
@@ -3381,7 +3378,7 @@
         <v>9</v>
       </c>
       <c r="E52" s="41" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3389,7 +3386,7 @@
         <v>105</v>
       </c>
       <c r="B53" s="12">
-        <f>(B52+1)</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C53" s="11" t="s">
@@ -3399,7 +3396,7 @@
         <v>9</v>
       </c>
       <c r="E53" s="41" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3407,7 +3404,7 @@
         <v>107</v>
       </c>
       <c r="B54" s="12">
-        <f>(B53+1)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="C54" s="11" t="s">
@@ -3425,7 +3422,7 @@
         <v>109</v>
       </c>
       <c r="B55" s="12">
-        <f>(B54+1)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C55" s="11" t="s">
@@ -3443,7 +3440,7 @@
         <v>111</v>
       </c>
       <c r="B56" s="12">
-        <f>(B55+1)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="C56" s="11" t="s">
@@ -3461,7 +3458,7 @@
         <v>113</v>
       </c>
       <c r="B57" s="12">
-        <f>(B56+1)</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="C57" s="11" t="s">
@@ -3471,7 +3468,7 @@
         <v>9</v>
       </c>
       <c r="E57" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3479,7 +3476,7 @@
         <v>115</v>
       </c>
       <c r="B58" s="12">
-        <f>(B57+1)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C58" s="11" t="s">
@@ -3489,7 +3486,7 @@
         <v>9</v>
       </c>
       <c r="E58" s="41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3497,7 +3494,7 @@
         <v>117</v>
       </c>
       <c r="B59" s="12">
-        <f>(B58+1)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="C59" s="11" t="s">
@@ -3507,7 +3504,7 @@
         <v>9</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3515,7 +3512,7 @@
         <v>119</v>
       </c>
       <c r="B60" s="12">
-        <f>(B59+1)</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -3525,7 +3522,7 @@
         <v>9</v>
       </c>
       <c r="E60" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3533,7 +3530,7 @@
         <v>121</v>
       </c>
       <c r="B61" s="12">
-        <f>(B60+1)</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="C61" s="11" t="s">
@@ -3543,7 +3540,7 @@
         <v>9</v>
       </c>
       <c r="E61" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3551,7 +3548,7 @@
         <v>123</v>
       </c>
       <c r="B62" s="12">
-        <f>(B61+1)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -3569,7 +3566,7 @@
         <v>125</v>
       </c>
       <c r="B63" s="12">
-        <f>(B62+1)</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="C63" s="11" t="s">
@@ -3587,7 +3584,7 @@
         <v>127</v>
       </c>
       <c r="B64" s="12">
-        <f>(B63+1)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="C64" s="11" t="s">
@@ -3605,7 +3602,7 @@
         <v>129</v>
       </c>
       <c r="B65" s="12">
-        <f>(B64+1)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C65" s="11" t="s">
@@ -3623,7 +3620,7 @@
         <v>131</v>
       </c>
       <c r="B66" s="12">
-        <f>(B65+1)</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="C66" s="11" t="s">
@@ -3633,7 +3630,7 @@
         <v>9</v>
       </c>
       <c r="E66" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3641,7 +3638,7 @@
         <v>133</v>
       </c>
       <c r="B67" s="12">
-        <f>(B66+1)</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="C67" s="11" t="s">
@@ -3659,7 +3656,7 @@
         <v>135</v>
       </c>
       <c r="B68" s="12">
-        <f>(B67+1)</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="C68" s="11" t="s">
@@ -3677,7 +3674,7 @@
         <v>137</v>
       </c>
       <c r="B69" s="12">
-        <f>(B68+1)</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="C69" s="11" t="s">
@@ -3691,11 +3688,11 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="45" t="s">
+      <c r="A70" s="43" t="s">
         <v>139</v>
       </c>
       <c r="B70" s="12">
-        <f>(B69+1)</f>
+        <f t="shared" ref="B70:B101" si="2">(B69+1)</f>
         <v>66</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -3713,7 +3710,7 @@
         <v>141</v>
       </c>
       <c r="B71" s="12">
-        <f>(B70+1)</f>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="C71" s="11" t="s">
@@ -3723,7 +3720,7 @@
         <v>9</v>
       </c>
       <c r="E71" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3731,7 +3728,7 @@
         <v>143</v>
       </c>
       <c r="B72" s="12">
-        <f>(B71+1)</f>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="C72" s="11" t="s">
@@ -3749,7 +3746,7 @@
         <v>145</v>
       </c>
       <c r="B73" s="12">
-        <f>(B72+1)</f>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="C73" s="11" t="s">
@@ -3767,7 +3764,7 @@
         <v>147</v>
       </c>
       <c r="B74" s="12">
-        <f>(B73+1)</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="C74" s="11" t="s">
@@ -3777,7 +3774,7 @@
         <v>9</v>
       </c>
       <c r="E74" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3785,7 +3782,7 @@
         <v>149</v>
       </c>
       <c r="B75" s="12">
-        <f>(B74+1)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="C75" s="11" t="s">
@@ -3795,7 +3792,7 @@
         <v>9</v>
       </c>
       <c r="E75" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3803,7 +3800,7 @@
         <v>151</v>
       </c>
       <c r="B76" s="12">
-        <f>(B75+1)</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="C76" s="11" t="s">
@@ -3813,7 +3810,7 @@
         <v>9</v>
       </c>
       <c r="E76" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3821,7 +3818,7 @@
         <v>153</v>
       </c>
       <c r="B77" s="12">
-        <f>(B76+1)</f>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="C77" s="11" t="s">
@@ -3831,7 +3828,7 @@
         <v>9</v>
       </c>
       <c r="E77" s="41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3839,7 +3836,7 @@
         <v>155</v>
       </c>
       <c r="B78" s="12">
-        <f>(B77+1)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="C78" s="11" t="s">
@@ -3849,7 +3846,7 @@
         <v>9</v>
       </c>
       <c r="E78" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3857,7 +3854,7 @@
         <v>157</v>
       </c>
       <c r="B79" s="12">
-        <f>(B78+1)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="C79" s="11" t="s">
@@ -3867,7 +3864,7 @@
         <v>9</v>
       </c>
       <c r="E79" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3875,7 +3872,7 @@
         <v>159</v>
       </c>
       <c r="B80" s="12">
-        <f>(B79+1)</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="C80" s="11" t="s">
@@ -3893,7 +3890,7 @@
         <v>161</v>
       </c>
       <c r="B81" s="12">
-        <f>(B80+1)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="C81" s="11" t="s">
@@ -3911,7 +3908,7 @@
         <v>163</v>
       </c>
       <c r="B82" s="12">
-        <f>(B81+1)</f>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="C82" s="11" t="s">
@@ -3921,7 +3918,7 @@
         <v>9</v>
       </c>
       <c r="E82" s="41" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
@@ -3929,7 +3926,7 @@
         <v>165</v>
       </c>
       <c r="B83" s="12">
-        <f>(B82+1)</f>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="C83" s="11" t="s">
@@ -3939,7 +3936,7 @@
         <v>9</v>
       </c>
       <c r="E83" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3947,7 +3944,7 @@
         <v>167</v>
       </c>
       <c r="B84" s="12">
-        <f>(B83+1)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="C84" s="11" t="s">
@@ -3965,7 +3962,7 @@
         <v>169</v>
       </c>
       <c r="B85" s="12">
-        <f>(B84+1)</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="C85" s="11" t="s">
@@ -3983,7 +3980,7 @@
         <v>171</v>
       </c>
       <c r="B86" s="12">
-        <f>(B85+1)</f>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="C86" s="11" t="s">
@@ -3993,15 +3990,15 @@
         <v>9</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="46" t="s">
+      <c r="A87" s="44" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="12">
-        <f>(B86+1)</f>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="C87" s="11" t="s">
@@ -4011,7 +4008,7 @@
         <v>9</v>
       </c>
       <c r="E87" s="41" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -4019,7 +4016,7 @@
         <v>175</v>
       </c>
       <c r="B88" s="12">
-        <f>(B87+1)</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="C88" s="11" t="s">
@@ -4029,7 +4026,7 @@
         <v>18</v>
       </c>
       <c r="E88" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4037,7 +4034,7 @@
         <v>177</v>
       </c>
       <c r="B89" s="12">
-        <f>(B88+1)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="C89" s="11" t="s">
@@ -4047,7 +4044,7 @@
         <v>9</v>
       </c>
       <c r="E89" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4055,7 +4052,7 @@
         <v>179</v>
       </c>
       <c r="B90" s="12">
-        <f>(B89+1)</f>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="C90" s="11" t="s">
@@ -4065,7 +4062,7 @@
         <v>9</v>
       </c>
       <c r="E90" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4073,7 +4070,7 @@
         <v>181</v>
       </c>
       <c r="B91" s="12">
-        <f>(B90+1)</f>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="C91" s="11" t="s">
@@ -4083,7 +4080,7 @@
         <v>18</v>
       </c>
       <c r="E91" s="41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4091,7 +4088,7 @@
         <v>183</v>
       </c>
       <c r="B92" s="12">
-        <f>(B91+1)</f>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="C92" s="11" t="s">
@@ -4101,7 +4098,7 @@
         <v>9</v>
       </c>
       <c r="E92" s="41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4109,7 +4106,7 @@
         <v>185</v>
       </c>
       <c r="B93" s="12">
-        <f>(B92+1)</f>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="C93" s="11" t="s">
@@ -4127,7 +4124,7 @@
         <v>187</v>
       </c>
       <c r="B94" s="12">
-        <f>(B93+1)</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="C94" s="11" t="s">
@@ -4137,7 +4134,7 @@
         <v>9</v>
       </c>
       <c r="E94" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4145,7 +4142,7 @@
         <v>189</v>
       </c>
       <c r="B95" s="12">
-        <f>(B94+1)</f>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="C95" s="11" t="s">
@@ -4155,7 +4152,7 @@
         <v>9</v>
       </c>
       <c r="E95" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4163,7 +4160,7 @@
         <v>191</v>
       </c>
       <c r="B96" s="12">
-        <f>(B95+1)</f>
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="C96" s="11" t="s">
@@ -4173,7 +4170,7 @@
         <v>9</v>
       </c>
       <c r="E96" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4181,7 +4178,7 @@
         <v>193</v>
       </c>
       <c r="B97" s="12">
-        <f>(B96+1)</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="C97" s="11" t="s">
@@ -4191,7 +4188,7 @@
         <v>9</v>
       </c>
       <c r="E97" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4199,7 +4196,7 @@
         <v>195</v>
       </c>
       <c r="B98" s="12">
-        <f>(B97+1)</f>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="C98" s="11" t="s">
@@ -4209,7 +4206,7 @@
         <v>9</v>
       </c>
       <c r="E98" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4217,7 +4214,7 @@
         <v>197</v>
       </c>
       <c r="B99" s="12">
-        <f>(B98+1)</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="C99" s="11" t="s">
@@ -4227,7 +4224,7 @@
         <v>9</v>
       </c>
       <c r="E99" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4235,7 +4232,7 @@
         <v>199</v>
       </c>
       <c r="B100" s="12">
-        <f>(B99+1)</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="C100" s="11" t="s">
@@ -4245,7 +4242,7 @@
         <v>9</v>
       </c>
       <c r="E100" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4253,7 +4250,7 @@
         <v>201</v>
       </c>
       <c r="B101" s="12">
-        <f>(B100+1)</f>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="C101" s="11" t="s">
@@ -4263,7 +4260,7 @@
         <v>9</v>
       </c>
       <c r="E101" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4271,7 +4268,7 @@
         <v>203</v>
       </c>
       <c r="B102" s="12">
-        <f>(B101+1)</f>
+        <f t="shared" ref="B102:B115" si="3">(B101+1)</f>
         <v>98</v>
       </c>
       <c r="C102" s="11" t="s">
@@ -4281,7 +4278,7 @@
         <v>9</v>
       </c>
       <c r="E102" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4289,7 +4286,7 @@
         <v>205</v>
       </c>
       <c r="B103" s="12">
-        <f>(B102+1)</f>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="C103" s="11" t="s">
@@ -4299,7 +4296,7 @@
         <v>9</v>
       </c>
       <c r="E103" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -4307,7 +4304,7 @@
         <v>207</v>
       </c>
       <c r="B104" s="12">
-        <f>(B103+1)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="C104" s="11" t="s">
@@ -4325,7 +4322,7 @@
         <v>209</v>
       </c>
       <c r="B105" s="12">
-        <f>(B104+1)</f>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="C105" s="11" t="s">
@@ -4335,7 +4332,7 @@
         <v>9</v>
       </c>
       <c r="E105" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4343,7 +4340,7 @@
         <v>211</v>
       </c>
       <c r="B106" s="12">
-        <f>(B105+1)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="C106" s="11" t="s">
@@ -4353,7 +4350,7 @@
         <v>9</v>
       </c>
       <c r="E106" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4361,7 +4358,7 @@
         <v>213</v>
       </c>
       <c r="B107" s="12">
-        <f>(B106+1)</f>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="C107" s="11" t="s">
@@ -4371,7 +4368,7 @@
         <v>9</v>
       </c>
       <c r="E107" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -4379,7 +4376,7 @@
         <v>215</v>
       </c>
       <c r="B108" s="12">
-        <f>(B107+1)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="C108" s="11" t="s">
@@ -4389,7 +4386,7 @@
         <v>9</v>
       </c>
       <c r="E108" s="41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4397,7 +4394,7 @@
         <v>217</v>
       </c>
       <c r="B109" s="12">
-        <f>(B108+1)</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="C109" s="11" t="s">
@@ -4415,7 +4412,7 @@
         <v>219</v>
       </c>
       <c r="B110" s="12">
-        <f>(B109+1)</f>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="C110" s="11" t="s">
@@ -4433,7 +4430,7 @@
         <v>221</v>
       </c>
       <c r="B111" s="12">
-        <f>(B110+1)</f>
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="C111" s="11" t="s">
@@ -4451,7 +4448,7 @@
         <v>223</v>
       </c>
       <c r="B112" s="12">
-        <f>(B111+1)</f>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="C112" s="11" t="s">
@@ -4469,7 +4466,7 @@
         <v>225</v>
       </c>
       <c r="B113" s="12">
-        <f>(B112+1)</f>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="C113" s="11" t="s">
@@ -4479,7 +4476,7 @@
         <v>9</v>
       </c>
       <c r="E113" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4487,7 +4484,7 @@
         <v>227</v>
       </c>
       <c r="B114" s="12">
-        <f>(B113+1)</f>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="C114" s="11" t="s">
@@ -4497,7 +4494,7 @@
         <v>9</v>
       </c>
       <c r="E114" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4505,7 +4502,7 @@
         <v>229</v>
       </c>
       <c r="B115" s="12">
-        <f>(B114+1)</f>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="C115" s="11" t="s">
@@ -4515,11 +4512,11 @@
         <v>9</v>
       </c>
       <c r="E115" s="41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A4:E115" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="E19:H19"/>
   </mergeCells>

</xml_diff>